<commit_message>
Add detailed experimental summary
Incorporate Excel analysis and update Kahan references
</commit_message>
<xml_diff>
--- a/dev-topics-algorithms/dev-topics-badaddr/analysis/addition_checker.xlsx
+++ b/dev-topics-algorithms/dev-topics-badaddr/analysis/addition_checker.xlsx
@@ -1238,11 +1238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55764096"/>
-        <c:axId val="123867136"/>
+        <c:axId val="123933440"/>
+        <c:axId val="123935744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55764096"/>
+        <c:axId val="123933440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1276,7 +1276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="123867136"/>
+        <c:crossAx val="123935744"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1287,7 +1287,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123867136"/>
+        <c:axId val="123935744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="17"/>
@@ -1330,7 +1330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55764096"/>
+        <c:crossAx val="123933440"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="BC105" sqref="BC105"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>